<commit_message>
agregue articulo 999 a 50 mil lucas en los dos excel
</commit_message>
<xml_diff>
--- a/LISTA NUEVA.xlsx
+++ b/LISTA NUEVA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupologisticoandreani-my.sharepoint.com/personal/mriccheri_andreani_com/Documents/Escritorio/FERRETEIA FC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupologisticoandreani-my.sharepoint.com/personal/mriccheri_andreani_com/Documents/Escritorio/FERRETEIA FC/VisualBasicFerre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="11_AD4D2F04E46CFB4ACB3E2073CD14FBD8683EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC788723-7C84-4F8D-A8BC-865BB2B9F7C7}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="11_AD4D2F04E46CFB4ACB3E2073CD14FBD8683EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8683DC6-93E2-48A2-B819-9C5C3C0F50AC}"/>
   <bookViews>
-    <workbookView xWindow="9885" yWindow="1170" windowWidth="12180" windowHeight="7740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="1605" windowWidth="12180" windowHeight="7740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NuevoPrecio" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>CAÑO 30 X 30</t>
+  </si>
+  <si>
+    <t>arma calibre 38</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,6 +670,20 @@
         <v>1242</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>999</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>50000</v>
+      </c>
+      <c r="D17" s="1">
+        <v>50000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
agregue listado nuevo en lista precios
</commit_message>
<xml_diff>
--- a/LISTA NUEVA.xlsx
+++ b/LISTA NUEVA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupologisticoandreani-my.sharepoint.com/personal/mriccheri_andreani_com/Documents/Escritorio/FERRETEIA FC/VisualBasicFerre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="11_AD4D2F04E46CFB4ACB3E2073CD14FBD8683EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8683DC6-93E2-48A2-B819-9C5C3C0F50AC}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="11_AD4D2F04E46CFB4ACB3E2073CD14FBD8683EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B27730CF-869D-429D-9AAF-EBC026400709}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="1605" windowWidth="12180" windowHeight="7740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NuevoPrecio" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -471,7 +471,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1">
-        <v>2000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -485,7 +485,7 @@
         <v>45</v>
       </c>
       <c r="D3" s="1">
-        <v>2354</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -499,7 +499,7 @@
         <v>45</v>
       </c>
       <c r="D4" s="1">
-        <v>2444</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
         <v>45</v>
       </c>
       <c r="D5" s="1">
-        <v>2566</v>
+        <v>220202</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>2888</v>
+        <v>202312</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -541,7 +541,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="1">
-        <v>2102</v>
+        <v>254454</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="1">
-        <v>2474</v>
+        <v>111111</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="1">
-        <v>2563</v>
+        <v>245120</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="1">
-        <v>2789</v>
+        <v>2012121</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="1">
-        <v>2222</v>
+        <v>12154</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,7 +611,7 @@
         <v>20</v>
       </c>
       <c r="D12" s="1">
-        <v>2410</v>
+        <v>12124</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="1">
-        <v>2012</v>
+        <v>121245</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>120</v>
       </c>
       <c r="D14" s="1">
-        <v>2232</v>
+        <v>121212</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="1">
-        <v>2031</v>
+        <v>1212451</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>1242</v>
       </c>
       <c r="D16" s="3">
-        <v>1242</v>
+        <v>12541854</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>50000</v>
       </c>
       <c r="D17" s="1">
-        <v>50000</v>
+        <v>500001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>